<commit_message>
I am just beginning to understand
</commit_message>
<xml_diff>
--- a/Excel_Challenge_561 - Maximum Profit.xlsx
+++ b/Excel_Challenge_561 - Maximum Profit.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A85F5C2-3702-4212-B5FD-C2C2333F16E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29051ED1-939B-4905-8241-B49A80621EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,8 +37,45 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="30">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -396,6 +434,64 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>13</v>
+    <v>3</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -657,6 +753,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="671" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{83354AD1-13EA-43A0-81C7-E31F451C8A73}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S11"/>
@@ -1105,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED62484-CB8B-480D-AFC8-91867FE2AC06}">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1220,6 +1343,10 @@
         <f>P3-O3</f>
         <v>64</v>
       </c>
+      <c r="S3" cm="1">
+        <f t="array" ref="S3:S11">_xlfn.BYROW(A3:J11,_xleta.MIN)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
@@ -1273,6 +1400,9 @@
         <f t="shared" ref="Q4:Q11" si="2">P4-O4</f>
         <v>74</v>
       </c>
+      <c r="S4">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
@@ -1326,6 +1456,9 @@
         <f t="shared" si="2"/>
         <v>87</v>
       </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
@@ -1379,6 +1512,9 @@
         <f t="shared" si="2"/>
         <v>69</v>
       </c>
+      <c r="S6">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
@@ -1432,6 +1568,9 @@
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
+      <c r="S7">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
@@ -1485,6 +1624,9 @@
         <f t="shared" si="2"/>
         <v>62</v>
       </c>
+      <c r="S8">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
@@ -1538,6 +1680,9 @@
         <f t="shared" si="2"/>
         <v>67</v>
       </c>
+      <c r="S9">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
@@ -1591,6 +1736,9 @@
         <f t="shared" si="2"/>
         <v>88</v>
       </c>
+      <c r="S10">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
@@ -1643,6 +1791,670 @@
       <c r="Q11">
         <f t="shared" si="2"/>
         <v>76</v>
+      </c>
+      <c r="S11">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE4F43C-EB5C-4CF4-A20C-2604B33C8C7B}">
+  <dimension ref="A1:S23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="6" width="4.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="4.33203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="4.33203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="6" customWidth="1"/>
+    <col min="12" max="12" width="5.5546875" customWidth="1"/>
+    <col min="13" max="13" width="6.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="S1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5">
+        <v>70</v>
+      </c>
+      <c r="C3" s="5">
+        <v>32</v>
+      </c>
+      <c r="D3" s="5">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5">
+        <v>19</v>
+      </c>
+      <c r="F3" s="5">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5">
+        <v>74</v>
+      </c>
+      <c r="H3" s="5">
+        <v>28</v>
+      </c>
+      <c r="I3" s="5">
+        <v>59</v>
+      </c>
+      <c r="J3" s="5">
+        <v>49</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>32</v>
+      </c>
+      <c r="B4" s="5">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5">
+        <v>31</v>
+      </c>
+      <c r="D4" s="5">
+        <v>59</v>
+      </c>
+      <c r="E4" s="5">
+        <v>7</v>
+      </c>
+      <c r="F4" s="5">
+        <v>70</v>
+      </c>
+      <c r="G4" s="5">
+        <v>46</v>
+      </c>
+      <c r="H4" s="5">
+        <v>81</v>
+      </c>
+      <c r="I4" s="5">
+        <v>17</v>
+      </c>
+      <c r="J4" s="5">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5">
+        <v>85</v>
+      </c>
+      <c r="D5" s="5">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5">
+        <v>81</v>
+      </c>
+      <c r="F5" s="5">
+        <v>75</v>
+      </c>
+      <c r="G5" s="5">
+        <v>35</v>
+      </c>
+      <c r="H5" s="5">
+        <v>10</v>
+      </c>
+      <c r="I5" s="5">
+        <v>89</v>
+      </c>
+      <c r="J5" s="5">
+        <v>91</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>87</v>
+      </c>
+      <c r="B6" s="5">
+        <v>87</v>
+      </c>
+      <c r="C6" s="5">
+        <v>87</v>
+      </c>
+      <c r="D6" s="5">
+        <v>87</v>
+      </c>
+      <c r="E6" s="5">
+        <v>87</v>
+      </c>
+      <c r="F6" s="5">
+        <v>80</v>
+      </c>
+      <c r="G6" s="5">
+        <v>74</v>
+      </c>
+      <c r="H6" s="5">
+        <v>45</v>
+      </c>
+      <c r="I6" s="5">
+        <v>26</v>
+      </c>
+      <c r="J6" s="5">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>93</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5">
+        <v>63</v>
+      </c>
+      <c r="E7" s="5">
+        <v>43</v>
+      </c>
+      <c r="F7" s="5">
+        <v>17</v>
+      </c>
+      <c r="G7" s="5">
+        <v>18</v>
+      </c>
+      <c r="H7" s="5">
+        <v>84</v>
+      </c>
+      <c r="I7" s="5">
+        <v>17</v>
+      </c>
+      <c r="J7" s="5">
+        <v>83</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>53</v>
+      </c>
+      <c r="B8" s="5">
+        <v>82</v>
+      </c>
+      <c r="C8" s="5">
+        <v>74</v>
+      </c>
+      <c r="D8" s="5">
+        <v>27</v>
+      </c>
+      <c r="E8" s="5">
+        <v>89</v>
+      </c>
+      <c r="F8" s="5">
+        <v>79</v>
+      </c>
+      <c r="G8" s="5">
+        <v>74</v>
+      </c>
+      <c r="H8" s="5">
+        <v>43</v>
+      </c>
+      <c r="I8" s="5">
+        <v>41</v>
+      </c>
+      <c r="J8" s="5">
+        <v>28</v>
+      </c>
+      <c r="K8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>59</v>
+      </c>
+      <c r="B9" s="5">
+        <v>63</v>
+      </c>
+      <c r="C9" s="5">
+        <v>16</v>
+      </c>
+      <c r="D9" s="5">
+        <v>34</v>
+      </c>
+      <c r="E9" s="5">
+        <v>44</v>
+      </c>
+      <c r="F9" s="5">
+        <v>21</v>
+      </c>
+      <c r="G9" s="5">
+        <v>4</v>
+      </c>
+      <c r="H9" s="5">
+        <v>71</v>
+      </c>
+      <c r="I9" s="5">
+        <v>36</v>
+      </c>
+      <c r="J9" s="5">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>96</v>
+      </c>
+      <c r="B10" s="5">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5">
+        <v>75</v>
+      </c>
+      <c r="D10" s="5">
+        <v>48</v>
+      </c>
+      <c r="E10" s="5">
+        <v>24</v>
+      </c>
+      <c r="F10" s="5">
+        <v>75</v>
+      </c>
+      <c r="G10" s="5">
+        <v>51</v>
+      </c>
+      <c r="H10" s="5">
+        <v>8</v>
+      </c>
+      <c r="I10" s="5">
+        <v>84</v>
+      </c>
+      <c r="J10" s="5">
+        <v>79</v>
+      </c>
+      <c r="K10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5">
+        <v>93</v>
+      </c>
+      <c r="C11" s="5">
+        <v>79</v>
+      </c>
+      <c r="D11" s="5">
+        <v>60</v>
+      </c>
+      <c r="E11" s="5">
+        <v>30</v>
+      </c>
+      <c r="F11" s="5">
+        <v>81</v>
+      </c>
+      <c r="G11" s="5">
+        <v>24</v>
+      </c>
+      <c r="H11" s="5">
+        <v>53</v>
+      </c>
+      <c r="I11" s="5">
+        <v>20</v>
+      </c>
+      <c r="J11" s="5">
+        <v>71</v>
+      </c>
+      <c r="K11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" cm="1">
+        <f t="array" ref="B15:D23">_xlfn.LET(
+    _xlpm.s, _xlfn.BYROW(
+        A3:J11,
+        _xlfn.LAMBDA(_xlpm.x, MAX(_xlfn.DROP(_xlpm.x, , _xlfn.XMATCH(MIN(_xlpm.x), _xlpm.x))))
+    ),
+    _xlpm.b, _xlfn.BYROW(A3:J11, _xleta.MIN),
+    IFERROR(_xlfn.HSTACK(_xlpm.b * _xlpm.s ^ 0, _xlpm.s, _xlpm.s - _xlpm.b), "NP")
+)</f>
+        <v>10</v>
+      </c>
+      <c r="C15" s="5">
+        <v>74</v>
+      </c>
+      <c r="D15" s="5">
+        <v>64</v>
+      </c>
+      <c r="G15" s="5" cm="1">
+        <f t="array" ref="G15:G23">_xlfn.LET(
+    _xlpm.s, _xlfn.BYROW(
+        A3:J11,
+        _xlfn.LAMBDA(_xlpm.x, MAX(_xlfn.DROP(_xlpm.x, , _xlfn.XMATCH(MIN(_xlpm.x), _xlpm.x))))
+    ),
+    _xlpm.b, _xlfn.BYROW(A3:J11, _xleta.MIN),
+    _xlpm.s
+)</f>
+        <v>74</v>
+      </c>
+      <c r="I15" s="5" cm="1">
+        <f t="array" ref="I15:I23">_xlfn.LET(
+    _xlpm.s, _xlfn.BYROW(
+        A3:J11,
+        _xlfn.LAMBDA(_xlpm.x, MAX(_xlfn.DROP(_xlpm.x, , _xlfn.XMATCH(MIN(_xlpm.x), _xlpm.x))))
+    ),
+    _xlpm.b, _xlfn.BYROW(A3:J11, _xleta.MIN),
+    _xlpm.b
+)</f>
+        <v>10</v>
+      </c>
+      <c r="K15" cm="1">
+        <f t="array" ref="K15:K23">_xlfn.LET(
+    _xlpm.s, _xlfn.BYROW(
+        A3:J11,
+        _xlfn.LAMBDA(_xlpm.x, MAX(_xlfn.DROP(_xlpm.x, , _xlfn.XMATCH(MIN(_xlpm.x), _xlpm.x))))
+    ),
+    _xlpm.s
+)</f>
+        <v>74</v>
+      </c>
+      <c r="M15">
+        <f>_xlfn.XMATCH(MIN(A6:J6),A6:J6)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B16" s="5">
+        <v>7</v>
+      </c>
+      <c r="C16" s="5">
+        <v>81</v>
+      </c>
+      <c r="D16" s="5">
+        <v>74</v>
+      </c>
+      <c r="G16" s="5">
+        <v>81</v>
+      </c>
+      <c r="I16" s="5">
+        <v>7</v>
+      </c>
+      <c r="K16">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="5">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5">
+        <v>91</v>
+      </c>
+      <c r="D17" s="5">
+        <v>87</v>
+      </c>
+      <c r="G17" s="5">
+        <v>91</v>
+      </c>
+      <c r="I17" s="5">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="str">
+        <v>NP</v>
+      </c>
+      <c r="C18" s="5" t="str">
+        <v>NP</v>
+      </c>
+      <c r="D18" s="5" t="str">
+        <v>NP</v>
+      </c>
+      <c r="G18" s="5" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I18" s="5">
+        <v>18</v>
+      </c>
+      <c r="K18" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="5">
+        <v>3</v>
+      </c>
+      <c r="C19" s="5">
+        <v>84</v>
+      </c>
+      <c r="D19" s="5">
+        <v>81</v>
+      </c>
+      <c r="G19" s="5">
+        <v>84</v>
+      </c>
+      <c r="I19" s="5">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="5">
+        <v>27</v>
+      </c>
+      <c r="C20" s="5">
+        <v>89</v>
+      </c>
+      <c r="D20" s="5">
+        <v>62</v>
+      </c>
+      <c r="G20" s="5">
+        <v>89</v>
+      </c>
+      <c r="I20" s="5">
+        <v>27</v>
+      </c>
+      <c r="K20">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="5">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5">
+        <v>71</v>
+      </c>
+      <c r="D21" s="5">
+        <v>67</v>
+      </c>
+      <c r="G21" s="5">
+        <v>71</v>
+      </c>
+      <c r="I21" s="5">
+        <v>4</v>
+      </c>
+      <c r="K21">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="5">
+        <v>8</v>
+      </c>
+      <c r="C22" s="5">
+        <v>84</v>
+      </c>
+      <c r="D22" s="5">
+        <v>76</v>
+      </c>
+      <c r="G22" s="5">
+        <v>84</v>
+      </c>
+      <c r="I22" s="5">
+        <v>8</v>
+      </c>
+      <c r="K22">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="5">
+        <v>17</v>
+      </c>
+      <c r="C23" s="5">
+        <v>93</v>
+      </c>
+      <c r="D23" s="5">
+        <v>76</v>
+      </c>
+      <c r="G23" s="5">
+        <v>93</v>
+      </c>
+      <c r="I23" s="5">
+        <v>17</v>
+      </c>
+      <c r="K23">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I figured out how to do a model. Good problem
</commit_message>
<xml_diff>
--- a/Excel_Challenge_561 - Maximum Profit.xlsx
+++ b/Excel_Challenge_561 - Maximum Profit.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29051ED1-939B-4905-8241-B49A80621EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BEC9BA-0622-4C25-8A97-3DAE4A1D29D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
+    <sheet name="EDA2" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="30">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -194,7 +195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,6 +214,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -226,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -242,6 +249,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,7 +765,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="671" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="407" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1228,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED62484-CB8B-480D-AFC8-91867FE2AC06}">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1807,7 +1817,7 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="B15" sqref="B15:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2461,4 +2471,1513 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E25EE03F-CC88-473C-9902-CC412458E067}">
+  <dimension ref="A1:Z40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="10" width="4.33203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="6" customWidth="1"/>
+    <col min="12" max="12" width="5.5546875" customWidth="1"/>
+    <col min="13" max="13" width="6.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="K1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="S1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5">
+        <v>70</v>
+      </c>
+      <c r="C3" s="5">
+        <v>32</v>
+      </c>
+      <c r="D3" s="5">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5">
+        <v>19</v>
+      </c>
+      <c r="F3" s="5">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5">
+        <v>74</v>
+      </c>
+      <c r="H3" s="5">
+        <v>28</v>
+      </c>
+      <c r="I3" s="5">
+        <v>59</v>
+      </c>
+      <c r="J3" s="5">
+        <v>49</v>
+      </c>
+      <c r="K3" s="9">
+        <v>10</v>
+      </c>
+      <c r="L3" s="9">
+        <v>74</v>
+      </c>
+      <c r="M3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>32</v>
+      </c>
+      <c r="B4" s="5">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5">
+        <v>31</v>
+      </c>
+      <c r="D4" s="5">
+        <v>59</v>
+      </c>
+      <c r="E4" s="5">
+        <v>7</v>
+      </c>
+      <c r="F4" s="5">
+        <v>70</v>
+      </c>
+      <c r="G4" s="5">
+        <v>46</v>
+      </c>
+      <c r="H4" s="5">
+        <v>81</v>
+      </c>
+      <c r="I4" s="5">
+        <v>17</v>
+      </c>
+      <c r="J4" s="5">
+        <v>12</v>
+      </c>
+      <c r="K4" s="9">
+        <v>7</v>
+      </c>
+      <c r="L4" s="9">
+        <v>81</v>
+      </c>
+      <c r="M4">
+        <v>74</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5">
+        <v>85</v>
+      </c>
+      <c r="D5" s="5">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5">
+        <v>81</v>
+      </c>
+      <c r="F5" s="5">
+        <v>75</v>
+      </c>
+      <c r="G5" s="5">
+        <v>35</v>
+      </c>
+      <c r="H5" s="5">
+        <v>10</v>
+      </c>
+      <c r="I5" s="5">
+        <v>89</v>
+      </c>
+      <c r="J5" s="5">
+        <v>91</v>
+      </c>
+      <c r="K5" s="9">
+        <v>4</v>
+      </c>
+      <c r="L5" s="9">
+        <v>91</v>
+      </c>
+      <c r="M5">
+        <v>87</v>
+      </c>
+      <c r="Q5" cm="1">
+        <f t="array" ref="Q5:Z5">INDEX(A3:J11,O4,)</f>
+        <v>51</v>
+      </c>
+      <c r="R5">
+        <v>70</v>
+      </c>
+      <c r="S5">
+        <v>32</v>
+      </c>
+      <c r="T5">
+        <v>10</v>
+      </c>
+      <c r="U5">
+        <v>19</v>
+      </c>
+      <c r="V5">
+        <v>13</v>
+      </c>
+      <c r="W5">
+        <v>74</v>
+      </c>
+      <c r="X5">
+        <v>28</v>
+      </c>
+      <c r="Y5">
+        <v>59</v>
+      </c>
+      <c r="Z5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>87</v>
+      </c>
+      <c r="B6" s="5">
+        <v>87</v>
+      </c>
+      <c r="C6" s="5">
+        <v>87</v>
+      </c>
+      <c r="D6" s="5">
+        <v>87</v>
+      </c>
+      <c r="E6" s="5">
+        <v>87</v>
+      </c>
+      <c r="F6" s="5">
+        <v>80</v>
+      </c>
+      <c r="G6" s="5">
+        <v>74</v>
+      </c>
+      <c r="H6" s="5">
+        <v>45</v>
+      </c>
+      <c r="I6" s="5">
+        <v>26</v>
+      </c>
+      <c r="J6" s="5">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" cm="1">
+        <f t="array" ref="P6:P15">TRANSPOSE(INDEX(A3:J11,O4,))</f>
+        <v>51</v>
+      </c>
+      <c r="Q6" cm="1">
+        <f t="array" ref="Q6:Z15">_xlfn.ANCHORARRAY(P6)-_xlfn.ANCHORARRAY(Q5)</f>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>-19</v>
+      </c>
+      <c r="S6">
+        <v>19</v>
+      </c>
+      <c r="T6">
+        <v>41</v>
+      </c>
+      <c r="U6">
+        <v>32</v>
+      </c>
+      <c r="V6">
+        <v>38</v>
+      </c>
+      <c r="W6">
+        <v>-23</v>
+      </c>
+      <c r="X6">
+        <v>23</v>
+      </c>
+      <c r="Y6">
+        <v>-8</v>
+      </c>
+      <c r="Z6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>93</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5">
+        <v>63</v>
+      </c>
+      <c r="E7" s="5">
+        <v>43</v>
+      </c>
+      <c r="F7" s="5">
+        <v>17</v>
+      </c>
+      <c r="G7" s="5">
+        <v>18</v>
+      </c>
+      <c r="H7" s="5">
+        <v>84</v>
+      </c>
+      <c r="I7" s="5">
+        <v>17</v>
+      </c>
+      <c r="J7" s="5">
+        <v>83</v>
+      </c>
+      <c r="K7" s="9">
+        <v>3</v>
+      </c>
+      <c r="L7" s="9">
+        <v>84</v>
+      </c>
+      <c r="M7">
+        <v>81</v>
+      </c>
+      <c r="P7">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>19</v>
+      </c>
+      <c r="R7" s="8">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>38</v>
+      </c>
+      <c r="T7">
+        <v>60</v>
+      </c>
+      <c r="U7">
+        <v>51</v>
+      </c>
+      <c r="V7">
+        <v>57</v>
+      </c>
+      <c r="W7">
+        <v>-4</v>
+      </c>
+      <c r="X7">
+        <v>42</v>
+      </c>
+      <c r="Y7">
+        <v>11</v>
+      </c>
+      <c r="Z7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>53</v>
+      </c>
+      <c r="B8" s="5">
+        <v>82</v>
+      </c>
+      <c r="C8" s="5">
+        <v>74</v>
+      </c>
+      <c r="D8" s="5">
+        <v>27</v>
+      </c>
+      <c r="E8" s="5">
+        <v>89</v>
+      </c>
+      <c r="F8" s="5">
+        <v>79</v>
+      </c>
+      <c r="G8" s="5">
+        <v>74</v>
+      </c>
+      <c r="H8" s="5">
+        <v>43</v>
+      </c>
+      <c r="I8" s="5">
+        <v>41</v>
+      </c>
+      <c r="J8" s="5">
+        <v>28</v>
+      </c>
+      <c r="K8" s="9">
+        <v>27</v>
+      </c>
+      <c r="L8" s="9">
+        <v>89</v>
+      </c>
+      <c r="M8">
+        <v>62</v>
+      </c>
+      <c r="P8">
+        <v>32</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>-19</v>
+      </c>
+      <c r="R8" s="7">
+        <v>-38</v>
+      </c>
+      <c r="S8" s="8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>22</v>
+      </c>
+      <c r="U8">
+        <v>13</v>
+      </c>
+      <c r="V8">
+        <v>19</v>
+      </c>
+      <c r="W8">
+        <v>-42</v>
+      </c>
+      <c r="X8">
+        <v>4</v>
+      </c>
+      <c r="Y8">
+        <v>-27</v>
+      </c>
+      <c r="Z8">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>59</v>
+      </c>
+      <c r="B9" s="5">
+        <v>63</v>
+      </c>
+      <c r="C9" s="5">
+        <v>16</v>
+      </c>
+      <c r="D9" s="5">
+        <v>34</v>
+      </c>
+      <c r="E9" s="5">
+        <v>44</v>
+      </c>
+      <c r="F9" s="5">
+        <v>21</v>
+      </c>
+      <c r="G9" s="5">
+        <v>4</v>
+      </c>
+      <c r="H9" s="5">
+        <v>71</v>
+      </c>
+      <c r="I9" s="5">
+        <v>36</v>
+      </c>
+      <c r="J9" s="5">
+        <v>64</v>
+      </c>
+      <c r="K9" s="9">
+        <v>4</v>
+      </c>
+      <c r="L9" s="9">
+        <v>71</v>
+      </c>
+      <c r="M9">
+        <v>67</v>
+      </c>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>-41</v>
+      </c>
+      <c r="R9" s="7">
+        <v>-60</v>
+      </c>
+      <c r="S9" s="7">
+        <v>-22</v>
+      </c>
+      <c r="T9" s="8">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>-9</v>
+      </c>
+      <c r="V9">
+        <v>-3</v>
+      </c>
+      <c r="W9">
+        <v>-64</v>
+      </c>
+      <c r="X9">
+        <v>-18</v>
+      </c>
+      <c r="Y9">
+        <v>-49</v>
+      </c>
+      <c r="Z9">
+        <v>-39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>96</v>
+      </c>
+      <c r="B10" s="5">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5">
+        <v>75</v>
+      </c>
+      <c r="D10" s="5">
+        <v>48</v>
+      </c>
+      <c r="E10" s="5">
+        <v>24</v>
+      </c>
+      <c r="F10" s="5">
+        <v>75</v>
+      </c>
+      <c r="G10" s="5">
+        <v>51</v>
+      </c>
+      <c r="H10" s="5">
+        <v>8</v>
+      </c>
+      <c r="I10" s="5">
+        <v>84</v>
+      </c>
+      <c r="J10" s="5">
+        <v>79</v>
+      </c>
+      <c r="K10" s="9">
+        <v>8</v>
+      </c>
+      <c r="L10" s="9">
+        <v>84</v>
+      </c>
+      <c r="M10">
+        <v>76</v>
+      </c>
+      <c r="P10">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>-32</v>
+      </c>
+      <c r="R10" s="7">
+        <v>-51</v>
+      </c>
+      <c r="S10" s="7">
+        <v>-13</v>
+      </c>
+      <c r="T10" s="7">
+        <v>9</v>
+      </c>
+      <c r="U10" s="8">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>6</v>
+      </c>
+      <c r="W10">
+        <v>-55</v>
+      </c>
+      <c r="X10">
+        <v>-9</v>
+      </c>
+      <c r="Y10">
+        <v>-40</v>
+      </c>
+      <c r="Z10">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5">
+        <v>93</v>
+      </c>
+      <c r="C11" s="5">
+        <v>79</v>
+      </c>
+      <c r="D11" s="5">
+        <v>60</v>
+      </c>
+      <c r="E11" s="5">
+        <v>30</v>
+      </c>
+      <c r="F11" s="5">
+        <v>81</v>
+      </c>
+      <c r="G11" s="5">
+        <v>24</v>
+      </c>
+      <c r="H11" s="5">
+        <v>53</v>
+      </c>
+      <c r="I11" s="5">
+        <v>20</v>
+      </c>
+      <c r="J11" s="5">
+        <v>71</v>
+      </c>
+      <c r="K11" s="9">
+        <v>17</v>
+      </c>
+      <c r="L11" s="9">
+        <v>93</v>
+      </c>
+      <c r="M11">
+        <v>76</v>
+      </c>
+      <c r="P11">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>-38</v>
+      </c>
+      <c r="R11" s="7">
+        <v>-57</v>
+      </c>
+      <c r="S11" s="7">
+        <v>-19</v>
+      </c>
+      <c r="T11" s="7">
+        <v>3</v>
+      </c>
+      <c r="U11" s="7">
+        <v>-6</v>
+      </c>
+      <c r="V11" s="8">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>-61</v>
+      </c>
+      <c r="X11">
+        <v>-15</v>
+      </c>
+      <c r="Y11">
+        <v>-46</v>
+      </c>
+      <c r="Z11">
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="P12">
+        <v>74</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>23</v>
+      </c>
+      <c r="R12" s="7">
+        <v>4</v>
+      </c>
+      <c r="S12" s="7">
+        <v>42</v>
+      </c>
+      <c r="T12" s="7">
+        <v>64</v>
+      </c>
+      <c r="U12" s="7">
+        <v>55</v>
+      </c>
+      <c r="V12" s="7">
+        <v>61</v>
+      </c>
+      <c r="W12" s="8">
+        <v>0</v>
+      </c>
+      <c r="X12" s="8">
+        <v>46</v>
+      </c>
+      <c r="Y12">
+        <v>15</v>
+      </c>
+      <c r="Z12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="P13">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>-23</v>
+      </c>
+      <c r="R13" s="7">
+        <v>-42</v>
+      </c>
+      <c r="S13" s="7">
+        <v>-4</v>
+      </c>
+      <c r="T13" s="7">
+        <v>18</v>
+      </c>
+      <c r="U13" s="7">
+        <v>9</v>
+      </c>
+      <c r="V13" s="7">
+        <v>15</v>
+      </c>
+      <c r="W13" s="7">
+        <v>-46</v>
+      </c>
+      <c r="X13" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>-31</v>
+      </c>
+      <c r="Z13">
+        <v>-21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="P14">
+        <v>59</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>8</v>
+      </c>
+      <c r="R14" s="7">
+        <v>-11</v>
+      </c>
+      <c r="S14" s="7">
+        <v>27</v>
+      </c>
+      <c r="T14" s="7">
+        <v>49</v>
+      </c>
+      <c r="U14" s="7">
+        <v>40</v>
+      </c>
+      <c r="V14" s="7">
+        <v>46</v>
+      </c>
+      <c r="W14" s="7">
+        <v>-15</v>
+      </c>
+      <c r="X14" s="7">
+        <v>31</v>
+      </c>
+      <c r="Y14" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="P15">
+        <v>49</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>-2</v>
+      </c>
+      <c r="R15" s="7">
+        <v>-21</v>
+      </c>
+      <c r="S15" s="7">
+        <v>17</v>
+      </c>
+      <c r="T15" s="7">
+        <v>39</v>
+      </c>
+      <c r="U15" s="7">
+        <v>30</v>
+      </c>
+      <c r="V15" s="7">
+        <v>36</v>
+      </c>
+      <c r="W15" s="7">
+        <v>-25</v>
+      </c>
+      <c r="X15" s="7">
+        <v>21</v>
+      </c>
+      <c r="Y15" s="7">
+        <v>-10</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="Q17" t="e">
+        <f>_xlfn.XMATCH($Q$29,Q18:Q27)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R17" t="e">
+        <f t="shared" ref="R17:Z17" si="0">_xlfn.XMATCH($Q$29,R18:R27)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S17" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="U17" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V17" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W17" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X17" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y17" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z17" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="P18" t="e">
+        <f>_xlfn.XMATCH($Q$29,Q18:Z18)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q18" cm="1">
+        <f t="array" ref="Q18:Z27">_xlfn.MAKEARRAY(10,10,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,IF(_xlpm.r&gt;_xlpm.c,INDEX(_xlfn.ANCHORARRAY(P6)-_xlfn.ANCHORARRAY(Q5),_xlpm.r,_xlpm.c),-1)))</f>
+        <v>-1</v>
+      </c>
+      <c r="R18">
+        <v>-1</v>
+      </c>
+      <c r="S18">
+        <v>-1</v>
+      </c>
+      <c r="T18">
+        <v>-1</v>
+      </c>
+      <c r="U18">
+        <v>-1</v>
+      </c>
+      <c r="V18">
+        <v>-1</v>
+      </c>
+      <c r="W18">
+        <v>-1</v>
+      </c>
+      <c r="X18">
+        <v>-1</v>
+      </c>
+      <c r="Y18">
+        <v>-1</v>
+      </c>
+      <c r="Z18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="P19" t="e">
+        <f t="shared" ref="P19:P27" si="1">_xlfn.XMATCH($Q$29,Q19:Z19)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q19">
+        <v>19</v>
+      </c>
+      <c r="R19">
+        <v>-1</v>
+      </c>
+      <c r="S19">
+        <v>-1</v>
+      </c>
+      <c r="T19">
+        <v>-1</v>
+      </c>
+      <c r="U19">
+        <v>-1</v>
+      </c>
+      <c r="V19">
+        <v>-1</v>
+      </c>
+      <c r="W19">
+        <v>-1</v>
+      </c>
+      <c r="X19">
+        <v>-1</v>
+      </c>
+      <c r="Y19">
+        <v>-1</v>
+      </c>
+      <c r="Z19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="P20" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q20">
+        <v>-19</v>
+      </c>
+      <c r="R20">
+        <v>-38</v>
+      </c>
+      <c r="S20">
+        <v>-1</v>
+      </c>
+      <c r="T20">
+        <v>-1</v>
+      </c>
+      <c r="U20">
+        <v>-1</v>
+      </c>
+      <c r="V20">
+        <v>-1</v>
+      </c>
+      <c r="W20">
+        <v>-1</v>
+      </c>
+      <c r="X20">
+        <v>-1</v>
+      </c>
+      <c r="Y20">
+        <v>-1</v>
+      </c>
+      <c r="Z20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="P21" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q21">
+        <v>-41</v>
+      </c>
+      <c r="R21">
+        <v>-60</v>
+      </c>
+      <c r="S21">
+        <v>-22</v>
+      </c>
+      <c r="T21">
+        <v>-1</v>
+      </c>
+      <c r="U21">
+        <v>-1</v>
+      </c>
+      <c r="V21">
+        <v>-1</v>
+      </c>
+      <c r="W21">
+        <v>-1</v>
+      </c>
+      <c r="X21">
+        <v>-1</v>
+      </c>
+      <c r="Y21">
+        <v>-1</v>
+      </c>
+      <c r="Z21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="P22" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q22">
+        <v>-32</v>
+      </c>
+      <c r="R22">
+        <v>-51</v>
+      </c>
+      <c r="S22">
+        <v>-13</v>
+      </c>
+      <c r="T22">
+        <v>9</v>
+      </c>
+      <c r="U22">
+        <v>-1</v>
+      </c>
+      <c r="V22">
+        <v>-1</v>
+      </c>
+      <c r="W22">
+        <v>-1</v>
+      </c>
+      <c r="X22">
+        <v>-1</v>
+      </c>
+      <c r="Y22">
+        <v>-1</v>
+      </c>
+      <c r="Z22">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="P23" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q23">
+        <v>-38</v>
+      </c>
+      <c r="R23">
+        <v>-57</v>
+      </c>
+      <c r="S23">
+        <v>-19</v>
+      </c>
+      <c r="T23">
+        <v>3</v>
+      </c>
+      <c r="U23">
+        <v>-6</v>
+      </c>
+      <c r="V23">
+        <v>-1</v>
+      </c>
+      <c r="W23">
+        <v>-1</v>
+      </c>
+      <c r="X23">
+        <v>-1</v>
+      </c>
+      <c r="Y23">
+        <v>-1</v>
+      </c>
+      <c r="Z23">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="P24">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Q24">
+        <v>23</v>
+      </c>
+      <c r="R24">
+        <v>4</v>
+      </c>
+      <c r="S24">
+        <v>42</v>
+      </c>
+      <c r="T24">
+        <v>64</v>
+      </c>
+      <c r="U24">
+        <v>55</v>
+      </c>
+      <c r="V24">
+        <v>61</v>
+      </c>
+      <c r="W24">
+        <v>-1</v>
+      </c>
+      <c r="X24">
+        <v>-1</v>
+      </c>
+      <c r="Y24">
+        <v>-1</v>
+      </c>
+      <c r="Z24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="P25" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q25">
+        <v>-23</v>
+      </c>
+      <c r="R25">
+        <v>-42</v>
+      </c>
+      <c r="S25">
+        <v>-4</v>
+      </c>
+      <c r="T25">
+        <v>18</v>
+      </c>
+      <c r="U25">
+        <v>9</v>
+      </c>
+      <c r="V25">
+        <v>15</v>
+      </c>
+      <c r="W25">
+        <v>-46</v>
+      </c>
+      <c r="X25">
+        <v>-1</v>
+      </c>
+      <c r="Y25">
+        <v>-1</v>
+      </c>
+      <c r="Z25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="P26" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q26">
+        <v>8</v>
+      </c>
+      <c r="R26">
+        <v>-11</v>
+      </c>
+      <c r="S26">
+        <v>27</v>
+      </c>
+      <c r="T26">
+        <v>49</v>
+      </c>
+      <c r="U26">
+        <v>40</v>
+      </c>
+      <c r="V26">
+        <v>46</v>
+      </c>
+      <c r="W26">
+        <v>-15</v>
+      </c>
+      <c r="X26">
+        <v>31</v>
+      </c>
+      <c r="Y26">
+        <v>-1</v>
+      </c>
+      <c r="Z26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="P27" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q27">
+        <v>-2</v>
+      </c>
+      <c r="R27">
+        <v>-21</v>
+      </c>
+      <c r="S27">
+        <v>17</v>
+      </c>
+      <c r="T27">
+        <v>39</v>
+      </c>
+      <c r="U27">
+        <v>30</v>
+      </c>
+      <c r="V27">
+        <v>36</v>
+      </c>
+      <c r="W27">
+        <v>-25</v>
+      </c>
+      <c r="X27">
+        <v>21</v>
+      </c>
+      <c r="Y27">
+        <v>-10</v>
+      </c>
+      <c r="Z27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="R28">
+        <f>LOOKUP(100,P18:P27,P18:P27)</f>
+        <v>4</v>
+      </c>
+      <c r="S28">
+        <f>LOOKUP(Q29,Q17:Y17,Q17:Y17)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="Q29" cm="1">
+        <f t="array" ref="Q29">_xlfn.LET(_xlpm.v,MAX(_xlfn.IFNA(_xlfn.ANCHORARRAY(Q18),-1)),IF(_xlpm.v=0,"NP",_xlpm.v))</f>
+        <v>64</v>
+      </c>
+      <c r="R29" cm="1">
+        <f t="array" ref="R29">INDEX($A$3:$J$11,$O$4,R28)</f>
+        <v>10</v>
+      </c>
+      <c r="S29" cm="1">
+        <f t="array" ref="S29">INDEX($A$3:$J$11,$O$4,S28)</f>
+        <v>74</v>
+      </c>
+      <c r="T29" t="str">
+        <f>_xlfn.TEXTJOIN(",",,R29,S29,Q29)</f>
+        <v>10,74,64</v>
+      </c>
+    </row>
+    <row r="31" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="Q31" t="str">
+        <f>T29</f>
+        <v>10,74,64</v>
+      </c>
+      <c r="R31" cm="1">
+        <f t="array" ref="R31:T31">_xlfn.IFNA(_xlfn.TEXTSPLIT(Q31,",")+0,{"NP","NP","NP"})</f>
+        <v>10</v>
+      </c>
+      <c r="S31">
+        <v>74</v>
+      </c>
+      <c r="T31">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="16:26" x14ac:dyDescent="0.3">
+      <c r="P32" cm="1">
+        <f t="array" ref="P32:P40">_xlfn.SEQUENCE(9)</f>
+        <v>1</v>
+      </c>
+      <c r="Q32" t="str">
+        <f t="dataTable" ref="Q32:Q40" dt2D="0" dtr="0" r1="O4"/>
+        <v>10,74,64</v>
+      </c>
+      <c r="R32" cm="1">
+        <f t="array" ref="R32:T32">_xlfn.IFNA(_xlfn.TEXTSPLIT(Q32,",")+0,{"NP","NP","NP"})</f>
+        <v>10</v>
+      </c>
+      <c r="S32">
+        <v>74</v>
+      </c>
+      <c r="T32">
+        <v>64</v>
+      </c>
+      <c r="V32" t="b" cm="1">
+        <f t="array" ref="V32:X40">R32:T40=K3:M11</f>
+        <v>1</v>
+      </c>
+      <c r="W32" t="b">
+        <v>1</v>
+      </c>
+      <c r="X32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="16:24" x14ac:dyDescent="0.3">
+      <c r="P33">
+        <v>2</v>
+      </c>
+      <c r="Q33" t="str">
+        <v>7,81,74</v>
+      </c>
+      <c r="R33" cm="1">
+        <f t="array" ref="R33:T33">_xlfn.IFNA(_xlfn.TEXTSPLIT(Q33,",")+0,{"NP","NP","NP"})</f>
+        <v>7</v>
+      </c>
+      <c r="S33">
+        <v>81</v>
+      </c>
+      <c r="T33">
+        <v>74</v>
+      </c>
+      <c r="V33" t="b">
+        <v>1</v>
+      </c>
+      <c r="W33" t="b">
+        <v>1</v>
+      </c>
+      <c r="X33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="16:24" x14ac:dyDescent="0.3">
+      <c r="P34">
+        <v>3</v>
+      </c>
+      <c r="Q34" t="str">
+        <v>4,91,87</v>
+      </c>
+      <c r="R34" cm="1">
+        <f t="array" ref="R34:T34">_xlfn.IFNA(_xlfn.TEXTSPLIT(Q34,",")+0,{"NP","NP","NP"})</f>
+        <v>4</v>
+      </c>
+      <c r="S34">
+        <v>91</v>
+      </c>
+      <c r="T34">
+        <v>87</v>
+      </c>
+      <c r="V34" t="b">
+        <v>1</v>
+      </c>
+      <c r="W34" t="b">
+        <v>1</v>
+      </c>
+      <c r="X34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="16:24" x14ac:dyDescent="0.3">
+      <c r="P35">
+        <v>4</v>
+      </c>
+      <c r="Q35" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R35" t="str" cm="1">
+        <f t="array" ref="R35:T35">_xlfn.IFNA(_xlfn.TEXTSPLIT(Q35,",")+0,{"NP","NP","NP"})</f>
+        <v>NP</v>
+      </c>
+      <c r="S35" t="str">
+        <v>NP</v>
+      </c>
+      <c r="T35" t="str">
+        <v>NP</v>
+      </c>
+      <c r="V35" t="b">
+        <v>1</v>
+      </c>
+      <c r="W35" t="b">
+        <v>1</v>
+      </c>
+      <c r="X35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="16:24" x14ac:dyDescent="0.3">
+      <c r="P36">
+        <v>5</v>
+      </c>
+      <c r="Q36" t="str">
+        <v>3,84,81</v>
+      </c>
+      <c r="R36" cm="1">
+        <f t="array" ref="R36:T36">_xlfn.IFNA(_xlfn.TEXTSPLIT(Q36,",")+0,{"NP","NP","NP"})</f>
+        <v>3</v>
+      </c>
+      <c r="S36">
+        <v>84</v>
+      </c>
+      <c r="T36">
+        <v>81</v>
+      </c>
+      <c r="V36" t="b">
+        <v>1</v>
+      </c>
+      <c r="W36" t="b">
+        <v>1</v>
+      </c>
+      <c r="X36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="16:24" x14ac:dyDescent="0.3">
+      <c r="P37">
+        <v>6</v>
+      </c>
+      <c r="Q37" t="str">
+        <v>27,89,62</v>
+      </c>
+      <c r="R37" cm="1">
+        <f t="array" ref="R37:T37">_xlfn.IFNA(_xlfn.TEXTSPLIT(Q37,",")+0,{"NP","NP","NP"})</f>
+        <v>27</v>
+      </c>
+      <c r="S37">
+        <v>89</v>
+      </c>
+      <c r="T37">
+        <v>62</v>
+      </c>
+      <c r="V37" t="b">
+        <v>1</v>
+      </c>
+      <c r="W37" t="b">
+        <v>1</v>
+      </c>
+      <c r="X37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="16:24" x14ac:dyDescent="0.3">
+      <c r="P38">
+        <v>7</v>
+      </c>
+      <c r="Q38" t="str">
+        <v>4,71,67</v>
+      </c>
+      <c r="R38" cm="1">
+        <f t="array" ref="R38:T38">_xlfn.IFNA(_xlfn.TEXTSPLIT(Q38,",")+0,{"NP","NP","NP"})</f>
+        <v>4</v>
+      </c>
+      <c r="S38">
+        <v>71</v>
+      </c>
+      <c r="T38">
+        <v>67</v>
+      </c>
+      <c r="V38" t="b">
+        <v>1</v>
+      </c>
+      <c r="W38" t="b">
+        <v>1</v>
+      </c>
+      <c r="X38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="16:24" x14ac:dyDescent="0.3">
+      <c r="P39">
+        <v>8</v>
+      </c>
+      <c r="Q39" t="str">
+        <v>8,84,76</v>
+      </c>
+      <c r="R39" cm="1">
+        <f t="array" ref="R39:T39">_xlfn.IFNA(_xlfn.TEXTSPLIT(Q39,",")+0,{"NP","NP","NP"})</f>
+        <v>8</v>
+      </c>
+      <c r="S39">
+        <v>84</v>
+      </c>
+      <c r="T39">
+        <v>76</v>
+      </c>
+      <c r="V39" t="b">
+        <v>1</v>
+      </c>
+      <c r="W39" t="b">
+        <v>1</v>
+      </c>
+      <c r="X39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="16:24" x14ac:dyDescent="0.3">
+      <c r="P40">
+        <v>9</v>
+      </c>
+      <c r="Q40" t="str">
+        <v>17,93,76</v>
+      </c>
+      <c r="R40" cm="1">
+        <f t="array" ref="R40:T40">_xlfn.IFNA(_xlfn.TEXTSPLIT(Q40,",")+0,{"NP","NP","NP"})</f>
+        <v>17</v>
+      </c>
+      <c r="S40">
+        <v>93</v>
+      </c>
+      <c r="T40">
+        <v>76</v>
+      </c>
+      <c r="V40" t="b">
+        <v>1</v>
+      </c>
+      <c r="W40" t="b">
+        <v>1</v>
+      </c>
+      <c r="X40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>